<commit_message>
ajustement du cahier des charges
Selon les critères d'évaluations
</commit_message>
<xml_diff>
--- a/analyse/base de données/dictionnaire de données/dictionnaire.xlsx
+++ b/analyse/base de données/dictionnaire de données/dictionnaire.xlsx
@@ -24,9 +24,6 @@
     <t>IDMess</t>
   </si>
   <si>
-    <t>Nom du champs</t>
-  </si>
-  <si>
     <t>Valeur défaut</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Equipe</t>
+  </si>
+  <si>
+    <t>Nom du champ</t>
   </si>
 </sst>
 </file>
@@ -276,13 +276,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -591,7 +591,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,900 +605,900 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3">
         <v>65535</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3">
         <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3">
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3">
         <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3">
         <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3">
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3">
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3">
         <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="A22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="3">
-        <v>10</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="3">
         <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="3">
         <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3">
         <v>30</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="3">
         <v>30</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="3">
         <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="3">
         <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="3">
         <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="3">
         <v>16</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="A47" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="3">
         <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1509,159 +1509,159 @@
         <v>65535</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
+      <c r="A54" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="7" t="s">
+      <c r="F55" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D56" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B57" s="3">
         <v>30</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="B60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="7" t="s">
+      <c r="F60" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D61" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B62" s="3">
         <v>30</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout d'un fichier sql pour bd
BD = MySQL
</commit_message>
<xml_diff>
--- a/analyse/base de données/dictionnaire de données/dictionnaire.xlsx
+++ b/analyse/base de données/dictionnaire de données/dictionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="58">
   <si>
     <t>Message</t>
   </si>
@@ -591,7 +591,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,11 +1295,11 @@
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>7</v>
+      <c r="B40" s="3">
+        <v>15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>16</v>

</xml_diff>